<commit_message>
More schematic changes + updated functionals
</commit_message>
<xml_diff>
--- a/Hardware/VNA/VNAbom.xlsx
+++ b/Hardware/VNA/VNAbom.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh Johnson\Dropbox\ENGN4200\vna\Hardware\VNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5B96EC63-9E9C-459F-92EC-9A5D4494B8A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5558278-17E4-44A5-890A-B8DDA04D7659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VNA" sheetId="1" r:id="rId1"/>
+    <sheet name="Digikey Order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="274">
   <si>
     <t>Item</t>
   </si>
@@ -142,9 +152,6 @@
     <t>Device:Polyfuse_Small</t>
   </si>
   <si>
-    <t>VNA_Footprints:Fuse_1206_3216Metric</t>
-  </si>
-  <si>
     <t>Bead</t>
   </si>
   <si>
@@ -337,12 +344,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
     <t>R26</t>
   </si>
   <si>
@@ -424,15 +425,6 @@
     <t>Package_DFN_QFN:DFN-6-1EP_2x2mm_P0.65mm_EP1x1.6mm</t>
   </si>
   <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>TVL755P</t>
-  </si>
-  <si>
-    <t>VNA_Symbols:TVL755P</t>
-  </si>
-  <si>
     <t>U6</t>
   </si>
   <si>
@@ -460,15 +452,6 @@
     <t>U8</t>
   </si>
   <si>
-    <t>PE43711</t>
-  </si>
-  <si>
-    <t>VNA_Symbols:PE43711</t>
-  </si>
-  <si>
-    <t>VNA_Footprints:QFN-24-1EP_4x4mm_P0.5mm_EP2.7x2.6mm_ThermalVias</t>
-  </si>
-  <si>
     <t>U9</t>
   </si>
   <si>
@@ -514,15 +497,6 @@
     <t>U14</t>
   </si>
   <si>
-    <t>PE4257</t>
-  </si>
-  <si>
-    <t>VNA_Symbols:PE4257</t>
-  </si>
-  <si>
-    <t>VNA_Footprints:QFN-20-1EP_4x4mm_P0.5mm_EP2.15x2.15mm_ThermalVias</t>
-  </si>
-  <si>
     <t>U15</t>
   </si>
   <si>
@@ -713,12 +687,177 @@
   </si>
   <si>
     <t>F921C105MPA</t>
+  </si>
+  <si>
+    <t>1276-1006-1-ND</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>1276-1184-2-ND</t>
+  </si>
+  <si>
+    <t>CL10B105KA8NNNC</t>
+  </si>
+  <si>
+    <t>490-5263-1-ND</t>
+  </si>
+  <si>
+    <t>BLM18PG181SN1D</t>
+  </si>
+  <si>
+    <t>0ZCK0050FF2E</t>
+  </si>
+  <si>
+    <t>507-1813-1-ND</t>
+  </si>
+  <si>
+    <t>VNA_Footprints:Fuse_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>RMCF0402JT16R0CT-ND</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>RMCF0402JT16R0</t>
+  </si>
+  <si>
+    <t>RMCF0603JT470RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT470R</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10K0</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT1K00CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT1K00</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00</t>
+  </si>
+  <si>
+    <t>RMCF0603ZT0R00TR-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT49R9CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT49R9</t>
+  </si>
+  <si>
+    <t>RMCF0402FT150RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT150R</t>
+  </si>
+  <si>
+    <t>RMCF0402FT60R4CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT60R4</t>
+  </si>
+  <si>
+    <t>RMCF0402JT39R0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402JT39R0</t>
+  </si>
+  <si>
+    <t>RMCF0402FT270RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT270R</t>
+  </si>
+  <si>
+    <t>RMCF0603JT1K50</t>
+  </si>
+  <si>
+    <t>RMCF0603JT1K50CT-ND</t>
+  </si>
+  <si>
+    <t>TPD2S017DBVR</t>
+  </si>
+  <si>
+    <t>296-25216-1-ND</t>
+  </si>
+  <si>
+    <t>LP5912Q3.3DRVRQ1</t>
+  </si>
+  <si>
+    <t>296-44294-1-ND</t>
+  </si>
+  <si>
+    <t>MIC5366-1.8YC5-TR</t>
+  </si>
+  <si>
+    <t>576-3203-1-ND</t>
+  </si>
+  <si>
+    <t>Mouser PN</t>
+  </si>
+  <si>
+    <t>296-37886-1-ND</t>
+  </si>
+  <si>
+    <t>TRF37A75IDSGT</t>
+  </si>
+  <si>
+    <t>1046-1038-1-ND</t>
+  </si>
+  <si>
+    <t>PE42440MLBB-Z</t>
+  </si>
+  <si>
+    <t>296-1090-1-ND</t>
+  </si>
+  <si>
+    <t>SN74AHC1G04DCKR</t>
+  </si>
+  <si>
+    <t>296-32297-1-ND</t>
+  </si>
+  <si>
+    <t>SN74LVC1G139DCUT</t>
+  </si>
+  <si>
+    <t>F2923NCGI</t>
+  </si>
+  <si>
+    <t>800-3575-ND</t>
+  </si>
+  <si>
+    <t>1265-1133-1-ND</t>
+  </si>
+  <si>
+    <t>AT25SF081-SSHD-T</t>
+  </si>
+  <si>
+    <t>535-12687-1-ND</t>
+  </si>
+  <si>
+    <t>ASTXR-12-19.200MHZ-512242-T</t>
+  </si>
+  <si>
+    <t>863-1298-1-ND</t>
+  </si>
+  <si>
+    <t>SKY12347-362LF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1552,11 +1691,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,11 +1707,11 @@
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1591,13 +1731,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="H1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="I1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1605,7 +1748,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1616,8 +1759,14 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1625,7 +1774,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1640,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1648,7 +1797,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1663,7 +1812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1671,7 +1820,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1686,7 +1835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1694,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1709,7 +1858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1717,7 +1866,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -1732,7 +1881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1755,7 +1904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1778,7 +1927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1786,7 +1935,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1797,8 +1946,14 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>222</v>
+      </c>
+      <c r="H10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1806,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -1821,7 +1976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1844,7 +1999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1852,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -1867,7 +2022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1890,7 +2045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1898,7 +2053,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -1913,7 +2068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1921,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -1944,7 +2099,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
         <v>27</v>
@@ -1956,10 +2111,10 @@
         <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="H17" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1970,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D18" t="s">
         <v>30</v>
@@ -2025,7 +2180,13 @@
         <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>227</v>
+      </c>
+      <c r="G20" t="s">
+        <v>225</v>
+      </c>
+      <c r="H20" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2036,16 +2197,22 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
         <v>41</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
-        <v>43</v>
+      <c r="G21" t="s">
+        <v>224</v>
+      </c>
+      <c r="H21" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2056,16 +2223,16 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
         <v>44</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>45</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
       </c>
       <c r="G22" t="s">
         <v>9</v>
@@ -2079,16 +2246,16 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
         <v>47</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>48</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>49</v>
-      </c>
-      <c r="F23" t="s">
-        <v>50</v>
       </c>
       <c r="G23" t="s">
         <v>9</v>
@@ -2102,16 +2269,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
         <v>51</v>
       </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
       <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
         <v>49</v>
-      </c>
-      <c r="F24" t="s">
-        <v>50</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
@@ -2125,16 +2292,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
         <v>53</v>
       </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
       <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
         <v>49</v>
-      </c>
-      <c r="F25" t="s">
-        <v>50</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
@@ -2148,16 +2315,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" t="s">
-        <v>56</v>
-      </c>
       <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
         <v>49</v>
-      </c>
-      <c r="F26" t="s">
-        <v>50</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
@@ -2171,22 +2338,22 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="D27" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="E27" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F27" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="G27" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H27" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2197,16 +2364,16 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
         <v>57</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>58</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>59</v>
-      </c>
-      <c r="F28" t="s">
-        <v>60</v>
       </c>
       <c r="G28" t="s">
         <v>9</v>
@@ -2220,16 +2387,16 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
         <v>61</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>62</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>63</v>
-      </c>
-      <c r="F29" t="s">
-        <v>64</v>
       </c>
       <c r="G29" t="s">
         <v>9</v>
@@ -2243,22 +2410,22 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
         <v>65</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>66</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>67</v>
       </c>
-      <c r="F30" t="s">
-        <v>68</v>
-      </c>
       <c r="G30" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="H30" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2269,16 +2436,16 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" t="s">
         <v>69</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>70</v>
-      </c>
-      <c r="F31" t="s">
-        <v>71</v>
       </c>
       <c r="G31" t="s">
         <v>9</v>
@@ -2292,16 +2459,16 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" t="s">
         <v>72</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>73</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>74</v>
-      </c>
-      <c r="F32" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2312,16 +2479,16 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
       </c>
       <c r="E33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" t="s">
         <v>77</v>
-      </c>
-      <c r="F33" t="s">
-        <v>78</v>
       </c>
       <c r="G33" t="s">
         <v>9</v>
@@ -2335,22 +2502,22 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s">
         <v>79</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>80</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>81</v>
       </c>
-      <c r="F34" t="s">
-        <v>82</v>
-      </c>
       <c r="G34" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="H34" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2361,16 +2528,22 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D35" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" t="s">
         <v>83</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>84</v>
       </c>
-      <c r="F35" t="s">
-        <v>85</v>
+      <c r="G35" t="s">
+        <v>232</v>
+      </c>
+      <c r="H35" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2381,16 +2554,16 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
         <v>86</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" t="s">
         <v>87</v>
-      </c>
-      <c r="E36" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" t="s">
-        <v>88</v>
       </c>
       <c r="G36" t="s">
         <v>9</v>
@@ -2404,16 +2577,22 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="G37" t="s">
+        <v>230</v>
+      </c>
+      <c r="H37" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2424,16 +2603,16 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" t="s">
         <v>90</v>
       </c>
-      <c r="D38" t="s">
-        <v>91</v>
-      </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" t="s">
         <v>9</v>
@@ -2447,16 +2626,16 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G39" t="s">
         <v>9</v>
@@ -2470,16 +2649,16 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40">
         <v>90.9</v>
       </c>
       <c r="E40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s">
         <v>9</v>
@@ -2493,16 +2672,16 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D41">
         <v>31.1</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G41" t="s">
         <v>9</v>
@@ -2516,16 +2695,16 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42">
         <v>240</v>
       </c>
       <c r="E42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s">
         <v>9</v>
@@ -2539,16 +2718,16 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43">
         <v>49.9</v>
       </c>
       <c r="E43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G43" t="s">
         <v>9</v>
@@ -2562,16 +2741,22 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F44" t="s">
         <v>84</v>
       </c>
-      <c r="F44" t="s">
-        <v>85</v>
+      <c r="G44" t="s">
+        <v>233</v>
+      </c>
+      <c r="H44" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -2582,16 +2767,22 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" t="s">
         <v>84</v>
       </c>
-      <c r="F45" t="s">
-        <v>85</v>
+      <c r="G45" t="s">
+        <v>236</v>
+      </c>
+      <c r="H45" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -2602,16 +2793,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" t="s">
         <v>98</v>
       </c>
-      <c r="D46" t="s">
-        <v>99</v>
-      </c>
       <c r="E46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G46" t="s">
         <v>9</v>
@@ -2625,16 +2816,16 @@
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D47">
         <v>52.3</v>
       </c>
       <c r="E47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G47" t="s">
         <v>9</v>
@@ -2648,22 +2839,22 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
         <v>101</v>
       </c>
-      <c r="D48" t="s">
-        <v>102</v>
-      </c>
       <c r="E48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2671,302 +2862,350 @@
         <v>1</v>
       </c>
       <c r="C49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" t="s">
         <v>103</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" t="s">
+        <v>83</v>
+      </c>
+      <c r="F50" t="s">
+        <v>84</v>
+      </c>
+      <c r="G50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
         <v>104</v>
       </c>
-      <c r="E49" t="s">
+      <c r="D51" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" t="s">
+        <v>87</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>197</v>
+      </c>
+      <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
+        <v>83</v>
+      </c>
+      <c r="F52" t="s">
         <v>84</v>
       </c>
-      <c r="F49" t="s">
-        <v>88</v>
-      </c>
-      <c r="G49" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" t="s">
-        <v>106</v>
-      </c>
-      <c r="E50" t="s">
-        <v>84</v>
-      </c>
-      <c r="F50" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51">
-        <v>2</v>
-      </c>
-      <c r="C51" t="s">
-        <v>208</v>
-      </c>
-      <c r="D51" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" t="s">
-        <v>84</v>
-      </c>
-      <c r="F51" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>107</v>
-      </c>
-      <c r="D52" t="s">
-        <v>108</v>
-      </c>
-      <c r="E52" t="s">
-        <v>84</v>
-      </c>
-      <c r="F52" t="s">
-        <v>88</v>
-      </c>
       <c r="G52" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="H52" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" t="s">
+        <v>83</v>
+      </c>
+      <c r="F53" t="s">
         <v>87</v>
       </c>
-      <c r="E53" t="s">
-        <v>84</v>
-      </c>
-      <c r="F53" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D54" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="E54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="H54" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D55" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" t="s">
+        <v>244</v>
+      </c>
+      <c r="H55" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D56" t="s">
         <v>109</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" t="s">
+        <v>87</v>
+      </c>
+      <c r="G56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E57" t="s">
+        <v>83</v>
+      </c>
+      <c r="F57" t="s">
+        <v>87</v>
+      </c>
+      <c r="G57" t="s">
+        <v>246</v>
+      </c>
+      <c r="H57" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" t="s">
+        <v>113</v>
+      </c>
+      <c r="E58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" t="s">
+        <v>87</v>
+      </c>
+      <c r="G58" t="s">
+        <v>248</v>
+      </c>
+      <c r="H58" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" t="s">
+        <v>83</v>
+      </c>
+      <c r="F59" t="s">
+        <v>87</v>
+      </c>
+      <c r="G59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>83</v>
+      </c>
+      <c r="F60" t="s">
         <v>84</v>
       </c>
-      <c r="F55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
+      <c r="G60" t="s">
+        <v>237</v>
+      </c>
+      <c r="H60" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>115</v>
+      </c>
+      <c r="D61" t="s">
+        <v>116</v>
+      </c>
+      <c r="E61" t="s">
+        <v>83</v>
+      </c>
+      <c r="F61" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" t="s">
+        <v>249</v>
+      </c>
+      <c r="H61" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" t="s">
+        <v>117</v>
+      </c>
+      <c r="E62" t="s">
+        <v>118</v>
+      </c>
+      <c r="F62" t="s">
+        <v>119</v>
+      </c>
+      <c r="G62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63">
         <v>2</v>
       </c>
-      <c r="C56" t="s">
-        <v>212</v>
-      </c>
-      <c r="D56" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" t="s">
-        <v>84</v>
-      </c>
-      <c r="F56" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" t="s">
-        <v>112</v>
-      </c>
-      <c r="E57" t="s">
-        <v>84</v>
-      </c>
-      <c r="F57" t="s">
-        <v>88</v>
-      </c>
-      <c r="G57" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>113</v>
-      </c>
-      <c r="D58" t="s">
-        <v>114</v>
-      </c>
-      <c r="E58" t="s">
-        <v>84</v>
-      </c>
-      <c r="F58" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>115</v>
-      </c>
-      <c r="D59" t="s">
-        <v>116</v>
-      </c>
-      <c r="E59" t="s">
-        <v>84</v>
-      </c>
-      <c r="F59" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>2</v>
-      </c>
-      <c r="C60" t="s">
-        <v>213</v>
-      </c>
-      <c r="D60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E60" t="s">
-        <v>84</v>
-      </c>
-      <c r="F60" t="s">
-        <v>88</v>
-      </c>
-      <c r="G60" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>8</v>
-      </c>
-      <c r="C61" t="s">
-        <v>214</v>
-      </c>
-      <c r="D61" t="s">
-        <v>112</v>
-      </c>
-      <c r="E61" t="s">
-        <v>84</v>
-      </c>
-      <c r="F61" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>118</v>
-      </c>
-      <c r="D62" t="s">
-        <v>119</v>
-      </c>
-      <c r="E62" t="s">
-        <v>84</v>
-      </c>
-      <c r="F62" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>3</v>
-      </c>
       <c r="C63" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D63" t="s">
         <v>120</v>
@@ -2978,366 +3217,896 @@
         <v>122</v>
       </c>
       <c r="G63" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="H63" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+      <c r="D64" t="s">
+        <v>124</v>
+      </c>
+      <c r="E64" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" t="s">
+        <v>126</v>
+      </c>
+      <c r="G64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65">
         <v>2</v>
       </c>
-      <c r="C64" t="s">
-        <v>216</v>
-      </c>
-      <c r="D64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E64" t="s">
-        <v>124</v>
-      </c>
-      <c r="F64" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
       <c r="C65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D65" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E65" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F65" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G65" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="H65" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D66" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E66" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F66" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="G66" t="s">
+        <v>255</v>
+      </c>
+      <c r="H66" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
       <c r="C67" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" t="s">
+        <v>138</v>
+      </c>
+      <c r="G67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>69</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" t="s">
+        <v>273</v>
+      </c>
+      <c r="G68" t="s">
+        <v>273</v>
+      </c>
+      <c r="H68" t="s">
+        <v>272</v>
+      </c>
+      <c r="I68" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" t="s">
+        <v>141</v>
+      </c>
+      <c r="E69" t="s">
+        <v>142</v>
+      </c>
+      <c r="F69" t="s">
+        <v>143</v>
+      </c>
+      <c r="G69" t="s">
+        <v>259</v>
+      </c>
+      <c r="H69" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>71</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>144</v>
+      </c>
+      <c r="D70" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" t="s">
+        <v>146</v>
+      </c>
+      <c r="F70" t="s">
         <v>134</v>
       </c>
-      <c r="D67" t="s">
-        <v>135</v>
-      </c>
-      <c r="E67" t="s">
-        <v>136</v>
-      </c>
-      <c r="F67" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" t="s">
-        <v>138</v>
-      </c>
-      <c r="E68" t="s">
-        <v>139</v>
-      </c>
-      <c r="F68" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" t="s">
-        <v>141</v>
-      </c>
-      <c r="D69" t="s">
-        <v>142</v>
-      </c>
-      <c r="E69" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" t="s">
-        <v>144</v>
-      </c>
-      <c r="G69" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" t="s">
-        <v>145</v>
-      </c>
-      <c r="D70" t="s">
-        <v>146</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="G70" t="s">
+        <v>263</v>
+      </c>
+      <c r="H70" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>72</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71" t="s">
         <v>147</v>
       </c>
-      <c r="F70" t="s">
+      <c r="E71" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="F71" t="s">
         <v>149</v>
       </c>
-      <c r="D71" t="s">
+      <c r="G71" t="s">
+        <v>261</v>
+      </c>
+      <c r="H71" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
         <v>150</v>
       </c>
-      <c r="E71" t="s">
+      <c r="D72" t="s">
         <v>151</v>
       </c>
-      <c r="F71" t="s">
+      <c r="E72" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="F72" t="s">
         <v>153</v>
       </c>
-      <c r="D72" t="s">
+      <c r="G72" t="s">
+        <v>265</v>
+      </c>
+      <c r="H72" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
         <v>154</v>
       </c>
-      <c r="E72" t="s">
+      <c r="D73" t="s">
+        <v>266</v>
+      </c>
+      <c r="G73" t="s">
+        <v>266</v>
+      </c>
+      <c r="H73" t="s">
+        <v>267</v>
+      </c>
+      <c r="I73" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
         <v>155</v>
       </c>
-      <c r="F72" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>2</v>
-      </c>
-      <c r="C73" t="s">
-        <v>217</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>156</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E74" t="s">
         <v>157</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F74" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="G74" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>76</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
         <v>159</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>160</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>161</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="G75" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>77</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
         <v>163</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>164</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>165</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F76" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="G76" t="s">
+        <v>269</v>
+      </c>
+      <c r="H76" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>78</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
         <v>167</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>168</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E77" t="s">
         <v>169</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F77" t="s">
         <v>170</v>
       </c>
-      <c r="G76" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="G77" t="s">
+        <v>271</v>
+      </c>
+      <c r="H77" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
         <v>171</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>172</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E78" t="s">
         <v>173</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F78" t="s">
         <v>174</v>
       </c>
-      <c r="G77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
-        <v>175</v>
-      </c>
-      <c r="D78" t="s">
-        <v>176</v>
-      </c>
-      <c r="E78" t="s">
-        <v>177</v>
-      </c>
-      <c r="F78" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-      <c r="C79" t="s">
-        <v>179</v>
-      </c>
-      <c r="D79" t="s">
-        <v>180</v>
-      </c>
-      <c r="E79" t="s">
-        <v>181</v>
-      </c>
-      <c r="F79" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>79</v>
-      </c>
+      <c r="G78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>1</v>
-      </c>
-      <c r="C80" t="s">
-        <v>183</v>
-      </c>
-      <c r="D80" t="s">
-        <v>184</v>
-      </c>
-      <c r="E80" t="s">
-        <v>185</v>
-      </c>
-      <c r="F80" t="s">
-        <v>186</v>
-      </c>
-      <c r="G80" t="s">
-        <v>9</v>
+        <f>SUM(B2:B78)</f>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{425E2ECF-0AE8-40C0-A631-047992CA1173}">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>240</v>
+      </c>
+      <c r="E13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>242</v>
+      </c>
+      <c r="E14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>248</v>
+      </c>
+      <c r="E17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" t="s">
+        <v>253</v>
+      </c>
+      <c r="E21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>273</v>
+      </c>
+      <c r="D23" t="s">
+        <v>273</v>
+      </c>
+      <c r="E23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>141</v>
+      </c>
+      <c r="C24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" t="s">
+        <v>259</v>
+      </c>
+      <c r="E24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" t="s">
+        <v>263</v>
+      </c>
+      <c r="E25" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" t="s">
+        <v>261</v>
+      </c>
+      <c r="E26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" t="s">
+        <v>265</v>
+      </c>
+      <c r="E27" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>266</v>
+      </c>
+      <c r="D28" t="s">
+        <v>266</v>
+      </c>
+      <c r="E28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" t="s">
+        <v>269</v>
+      </c>
+      <c r="E29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>